<commit_message>
Iss #5 implement dead zone support in Rotator
</commit_message>
<xml_diff>
--- a/Gear and Step Calculator.xlsx
+++ b/Gear and Step Calculator.xlsx
@@ -1,32 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\source\repos\TA.NexDome\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDAC541D-ACEA-4060-82E9-286E79E2830D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC09E16-B80A-4EA5-8A5D-A36F51C543F0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27675" yWindow="1170" windowWidth="25890" windowHeight="12945" xr2:uid="{6850C48A-CC6E-469D-8432-6E56DCA5654D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{25697728-F04A-4FF6-8584-528B5258E361}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Rotator" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Degrees_Per_Step">Sheet1!$B$7</definedName>
-    <definedName name="Gearbox_Reduction">Sheet1!$B$6</definedName>
-    <definedName name="Microsteps_Per_Step">Sheet1!$B$5</definedName>
-    <definedName name="Pinion_Rotations_Per_Rack_Rotation">Sheet1!$B$8</definedName>
-    <definedName name="Rotator_Pinion_Teeth">Sheet1!$B$4</definedName>
-    <definedName name="Rotator_Rack_Teeth">Sheet1!$B$3</definedName>
-    <definedName name="Whole_Steps_Per_Motor_Revolution">Sheet1!$B$9</definedName>
-    <definedName name="Whole_Steps_Per_Pinion_Revolution">Sheet1!$B$10</definedName>
-    <definedName name="Whole_Steps_Per_Rack_Rotation">Sheet1!$B$11</definedName>
+    <definedName name="Computed_Properties">Rotator!$B$16</definedName>
+    <definedName name="Final_Output_Steps_per_Rotation">Rotator!$B$13</definedName>
+    <definedName name="Full_Steps_Per_Degree_Azimuth">Rotator!$B$19</definedName>
+    <definedName name="Full_Steps_Per_Dome_Rotation">Rotator!$B$17</definedName>
+    <definedName name="Gearbox">Rotator!$B$11</definedName>
+    <definedName name="Gearbox_Reduction">Rotator!$B$11</definedName>
+    <definedName name="Geared_step_angle">Rotator!$B$12</definedName>
+    <definedName name="Microsteps_per_Dome_Rotation">Rotator!$B$18</definedName>
+    <definedName name="Microsteps_per_Step">Rotator!$B$14</definedName>
+    <definedName name="Motor_and_Gearbox">Rotator!$B$8</definedName>
+    <definedName name="NexDome_Hardware">Rotator!$B$3</definedName>
+    <definedName name="Pinion_Rotations_per_Dome_Rotation">Rotator!$B$6</definedName>
+    <definedName name="Pinion_Teeth">Rotator!$B$5</definedName>
+    <definedName name="Rack_Teeth">Rotator!$B$4</definedName>
+    <definedName name="Raw_step_angle">Rotator!$B$9</definedName>
+    <definedName name="Steps_per_rotation">Rotator!$B$10</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,50 +48,138 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Tim Long</author>
+  </authors>
+  <commentList>
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{B2FAB134-D771-4EE3-B79E-E0D1DD40CD24}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tim Long:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+https://www.phidgets.com/?tier=3&amp;catid=24&amp;pcid=21&amp;prodid=352</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A12" authorId="0" shapeId="0" xr:uid="{C6CA3BF8-AC87-4330-9BE8-702325086DCB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tim Long:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+per data sheet: "When using the step angle in calculations, you should derive the exact step angle by dividing 1.8° by the gearbox reduction ratio."</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Rotator Rack Teeth</t>
-  </si>
-  <si>
-    <t>Rotator Pinion Teeth</t>
-  </si>
-  <si>
-    <t>Microsteps Per Step</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+  <si>
+    <t>NexDome Hardware</t>
+  </si>
+  <si>
+    <t>Rack Teeth</t>
+  </si>
+  <si>
+    <t>(assumption: rack extends 360 degrees)</t>
+  </si>
+  <si>
+    <t>Pinion Teeth</t>
+  </si>
+  <si>
+    <t>Pinion Rotations per Dome Rotation</t>
+  </si>
+  <si>
+    <t>Motor and Gearbox</t>
+  </si>
+  <si>
+    <t>Raw step angle</t>
+  </si>
+  <si>
+    <t>°</t>
+  </si>
+  <si>
+    <t>Steps per rotation</t>
+  </si>
+  <si>
+    <t>whole steps per motor input shaft rotation</t>
   </si>
   <si>
     <t>Gearbox Reduction</t>
   </si>
   <si>
-    <t>:1</t>
-  </si>
-  <si>
-    <t>Pinion Rotations Per Rack Rotation</t>
-  </si>
-  <si>
-    <t>Degrees Per Step</t>
-  </si>
-  <si>
-    <t>steps per rotation</t>
-  </si>
-  <si>
-    <t>Whole Steps Per Motor Revolution</t>
-  </si>
-  <si>
-    <t>Whole Steps Per Pinion Revolution</t>
-  </si>
-  <si>
-    <t>Whole Steps Per Rack Rotation</t>
-  </si>
-  <si>
-    <t>Microsteps Per Rack Rotation</t>
+    <t>:1 reduction (from data sheet)</t>
+  </si>
+  <si>
+    <t>Geared step angle</t>
+  </si>
+  <si>
+    <t>°/step</t>
+  </si>
+  <si>
+    <t>Final Output Steps per Rotation</t>
+  </si>
+  <si>
+    <t>Microsteps per Step</t>
+  </si>
+  <si>
+    <t>(selectable, 8 is the default)</t>
+  </si>
+  <si>
+    <t>Computed Properties</t>
+  </si>
+  <si>
+    <t>Full Steps Per Dome Rotation</t>
+  </si>
+  <si>
+    <t>Microsteps per Dome Rotation</t>
+  </si>
+  <si>
+    <t>Full Steps Per Degree Azimuth</t>
+  </si>
+  <si>
+    <t>Microsteps Per Degree Azimuth</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,16 +187,62 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -109,14 +250,47 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Calculation" xfId="3" builtinId="22"/>
+    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
+    <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -428,115 +602,172 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2BEE2FB-BCC4-4675-AAB9-E2A74D1D907D}">
-  <dimension ref="A3:E12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9B73FE4-1D52-4431-B137-6BAD080B4A14}">
+  <dimension ref="A3:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="1" max="1" width="36.42578125" customWidth="1"/>
+    <col min="3" max="3" width="39.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
+        <v>288</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <f>Rack_Teeth/Pinion_Teeth</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>1.8</v>
-      </c>
-      <c r="D7">
-        <f>360/B7</f>
+      <c r="B10" s="2">
+        <f>360/Raw_step_angle</f>
         <v>200</v>
       </c>
-      <c r="E7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <f>Rotator_Rack_Teeth/Rotator_Pinion_Teeth</f>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <f>360/Degrees_Per_Step</f>
-        <v>200</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C10" t="s">
         <v>9</v>
       </c>
-      <c r="B10">
-        <f>Whole_Steps_Per_Motor_Revolution*Gearbox_Reduction</f>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11">
-        <f>Whole_Steps_Per_Pinion_Revolution*Pinion_Rotations_Per_Rack_Rotation</f>
-        <v>54000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="3">
+        <v>15.3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <f>Whole_Steps_Per_Rack_Rotation*Microsteps_Per_Step</f>
-        <v>432000</v>
+        <v>12</v>
+      </c>
+      <c r="B12" s="2">
+        <f>Raw_step_angle/Gearbox_Reduction</f>
+        <v>0.11764705882352941</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="2">
+        <f>360/Geared_step_angle</f>
+        <v>3060</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="3">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="2">
+        <f>Pinion_Rotations_per_Dome_Rotation*Final_Output_Steps_per_Rotation</f>
+        <v>55080</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="2">
+        <f>Full_Steps_Per_Dome_Rotation*Microsteps_per_Step</f>
+        <v>440640</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="2">
+        <f>Full_Steps_Per_Dome_Rotation/360</f>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="2">
+        <f>Microsteps_per_Dome_Rotation/360</f>
+        <v>1224</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>